<commit_message>
Changed hardcoded absolute paths into environment-independent relative paths
</commit_message>
<xml_diff>
--- a/dice_scores.xlsx
+++ b/dice_scores.xlsx
@@ -480,13 +480,13 @@
         </is>
       </c>
       <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
         <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -504,13 +504,13 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -528,13 +528,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -552,13 +552,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -576,10 +576,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>2</v>
@@ -600,13 +600,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E7" t="n">
         <v>2</v>
       </c>
       <c r="F7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -624,10 +624,10 @@
         </is>
       </c>
       <c r="D8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" t="n">
         <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>6</v>
@@ -672,13 +672,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -696,13 +696,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" t="n">
         <v>7</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -720,13 +720,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
@@ -744,13 +744,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
@@ -768,13 +768,13 @@
         </is>
       </c>
       <c r="D14" t="n">
+        <v>10</v>
+      </c>
+      <c r="E14" t="n">
         <v>7</v>
       </c>
-      <c r="E14" t="n">
-        <v>5</v>
-      </c>
       <c r="F14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -792,13 +792,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
@@ -819,10 +819,10 @@
         <v>5</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -840,13 +840,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="n">
         <v>7</v>
-      </c>
-      <c r="F17" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -864,13 +864,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E18" t="n">
         <v>9</v>
       </c>
       <c r="F18" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -888,10 +888,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>8</v>
@@ -912,13 +912,13 @@
         </is>
       </c>
       <c r="D20" t="n">
+        <v>6</v>
+      </c>
+      <c r="E20" t="n">
         <v>0</v>
       </c>
-      <c r="E20" t="n">
-        <v>4</v>
-      </c>
       <c r="F20" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -936,13 +936,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added relative paths for older code too + improved graphs
</commit_message>
<xml_diff>
--- a/dice_scores.xlsx
+++ b/dice_scores.xlsx
@@ -480,10 +480,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -504,13 +504,13 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -528,13 +528,13 @@
         </is>
       </c>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
         <v>10</v>
       </c>
-      <c r="E4" t="n">
-        <v>5</v>
-      </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -552,13 +552,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" t="n">
         <v>5</v>
-      </c>
-      <c r="F5" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -579,10 +579,10 @@
         <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -600,13 +600,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -627,10 +627,10 @@
         <v>4</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -648,13 +648,13 @@
         </is>
       </c>
       <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
         <v>6</v>
       </c>
-      <c r="E9" t="n">
-        <v>9</v>
-      </c>
       <c r="F9" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -672,13 +672,13 @@
         </is>
       </c>
       <c r="D10" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
         <v>10</v>
-      </c>
-      <c r="E10" t="n">
-        <v>4</v>
-      </c>
-      <c r="F10" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -696,13 +696,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -723,10 +723,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -744,13 +744,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -768,13 +768,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -792,13 +792,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -816,13 +816,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
@@ -840,13 +840,13 @@
         </is>
       </c>
       <c r="D17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4</v>
+      </c>
+      <c r="F17" t="n">
         <v>8</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="18">
@@ -864,13 +864,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -888,13 +888,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -915,7 +915,7 @@
         <v>6</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>2</v>
@@ -936,13 +936,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a scenario to dobbelsteen.py
</commit_message>
<xml_diff>
--- a/dice_scores.xlsx
+++ b/dice_scores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,31 @@
           <t>Round_3</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Round_4</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Round_5</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Round_6</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Round_7</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Round_8</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -476,17 +501,32 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Majis</t>
+          <t>Pocky Lovers</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E2" t="n">
+        <v>7</v>
+      </c>
+      <c r="F2" t="n">
         <v>9</v>
       </c>
-      <c r="F2" t="n">
-        <v>1</v>
+      <c r="G2" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2" t="n">
+        <v>9</v>
+      </c>
+      <c r="J2" t="n">
+        <v>10</v>
+      </c>
+      <c r="K2" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -500,23 +540,38 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Majis</t>
+          <t>Pocky Lovers</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>4</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kiryu</t>
+          <t>Cyber</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -524,16 +579,31 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dragon Team</t>
+          <t>Chocolate Lovers</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E4" t="n">
         <v>10</v>
       </c>
       <c r="F4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" t="n">
+        <v>9</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>10</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" t="n">
         <v>6</v>
       </c>
     </row>
@@ -548,17 +618,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Majis</t>
+          <t>Chocolate Lovers</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G5" t="n">
         <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>7</v>
+      </c>
+      <c r="I5" t="n">
+        <v>6</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K5" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -572,377 +657,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Majis</t>
+          <t>Pocky Lovers</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Cyber</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Majis</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>9</v>
-      </c>
-      <c r="E7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F7" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
         <v>7</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Yamai</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Baddies</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" t="n">
-        <v>7</v>
-      </c>
-      <c r="F8" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Sasaki</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
         <v>8</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Baddies</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F9" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Okita</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Japanese Plushies</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>9</v>
-      </c>
-      <c r="E10" t="n">
-        <v>2</v>
-      </c>
-      <c r="F10" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Ryoma</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>10</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Japanese Plushies</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>10</v>
-      </c>
-      <c r="E11" t="n">
-        <v>2</v>
-      </c>
-      <c r="F11" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Saejima</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>11</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Hydrogenpink Plushies</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>10</v>
-      </c>
-      <c r="E12" t="n">
-        <v>7</v>
-      </c>
-      <c r="F12" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Nagakura</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>12</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Japanese Plushies</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" t="n">
-        <v>4</v>
-      </c>
-      <c r="F13" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Futaba</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>13</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Phantom Thieves</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>7</v>
-      </c>
-      <c r="E14" t="n">
-        <v>6</v>
-      </c>
-      <c r="F14" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Jokah</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>14</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Phantom Thieves</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" t="n">
-        <v>9</v>
-      </c>
-      <c r="F15" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Star</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>15</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Japanese Plushies</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>6</v>
-      </c>
-      <c r="E16" t="n">
-        <v>2</v>
-      </c>
-      <c r="F16" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Majima</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>16</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Hydrogenpink Plushies</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>2</v>
-      </c>
-      <c r="E17" t="n">
-        <v>4</v>
-      </c>
-      <c r="F17" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Karola</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>17</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>House Lady</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Nishitani</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>18</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Baddies</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>5</v>
-      </c>
-      <c r="E19" t="n">
-        <v>7</v>
-      </c>
-      <c r="F19" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Bunchan</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>19</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Japanese Plushies</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>6</v>
-      </c>
-      <c r="E20" t="n">
-        <v>4</v>
-      </c>
-      <c r="F20" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Kirby</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>20</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Japanese Plushies</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>2</v>
-      </c>
-      <c r="E21" t="n">
+      <c r="K6" t="n">
         <v>0</v>
-      </c>
-      <c r="F21" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made y-axis range dynamic
</commit_message>
<xml_diff>
--- a/dice_scores.xlsx
+++ b/dice_scores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,16 +479,6 @@
           <t>Round_6</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Round_7</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Round_8</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -505,28 +495,22 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
       </c>
       <c r="F2" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2" t="n">
         <v>7</v>
-      </c>
-      <c r="H2" t="n">
-        <v>8</v>
-      </c>
-      <c r="I2" t="n">
-        <v>9</v>
-      </c>
-      <c r="J2" t="n">
-        <v>10</v>
-      </c>
-      <c r="K2" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -547,25 +531,19 @@
         <v>7</v>
       </c>
       <c r="E3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" t="n">
         <v>4</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -583,28 +561,22 @@
         </is>
       </c>
       <c r="D4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>9</v>
+      </c>
+      <c r="G4" t="n">
         <v>8</v>
       </c>
-      <c r="E4" t="n">
-        <v>10</v>
-      </c>
-      <c r="F4" t="n">
-        <v>4</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" t="n">
         <v>9</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>10</v>
-      </c>
-      <c r="J4" t="n">
-        <v>2</v>
-      </c>
-      <c r="K4" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -625,25 +597,19 @@
         <v>1</v>
       </c>
       <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" t="n">
         <v>5</v>
-      </c>
-      <c r="F5" t="n">
-        <v>7</v>
-      </c>
-      <c r="G5" t="n">
-        <v>5</v>
-      </c>
-      <c r="H5" t="n">
-        <v>7</v>
-      </c>
-      <c r="I5" t="n">
-        <v>6</v>
-      </c>
-      <c r="J5" t="n">
-        <v>3</v>
-      </c>
-      <c r="K5" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -661,28 +627,22 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
+        <v>7</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" t="n">
         <v>6</v>
       </c>
-      <c r="F6" t="n">
-        <v>4</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>7</v>
-      </c>
       <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>8</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Just to be sure
</commit_message>
<xml_diff>
--- a/dice_scores.xlsx
+++ b/dice_scores.xlsx
@@ -495,22 +495,22 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
         <v>2</v>
       </c>
-      <c r="G2" t="n">
-        <v>6</v>
-      </c>
-      <c r="H2" t="n">
-        <v>6</v>
-      </c>
       <c r="I2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>9</v>
+      </c>
+      <c r="F4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G4" t="n">
         <v>7</v>
       </c>
-      <c r="E4" t="n">
-        <v>5</v>
-      </c>
-      <c r="F4" t="n">
-        <v>9</v>
-      </c>
-      <c r="G4" t="n">
-        <v>8</v>
-      </c>
       <c r="H4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -594,22 +594,22 @@
         </is>
       </c>
       <c r="D5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G5" t="n">
         <v>1</v>
       </c>
-      <c r="E5" t="n">
+      <c r="H5" t="n">
         <v>2</v>
       </c>
-      <c r="F5" t="n">
-        <v>4</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>3</v>
-      </c>
       <c r="I5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -627,22 +627,22 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" t="n">
         <v>7</v>
       </c>
-      <c r="F6" t="n">
-        <v>5</v>
-      </c>
-      <c r="G6" t="n">
-        <v>2</v>
-      </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>6</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned the code and made user prompts defensive
</commit_message>
<xml_diff>
--- a/dice_scores.xlsx
+++ b/dice_scores.xlsx
@@ -480,13 +480,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -504,13 +504,13 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -528,13 +528,13 @@
         </is>
       </c>
       <c r="D4" t="n">
+        <v>9</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="n">
         <v>4</v>
-      </c>
-      <c r="E4" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -552,13 +552,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -576,13 +576,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some first more relevant tables and piping them to Word doc
</commit_message>
<xml_diff>
--- a/dice_scores.xlsx
+++ b/dice_scores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,16 @@
           <t>Round_3</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Round_4</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Round_5</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -480,13 +490,19 @@
         </is>
       </c>
       <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
         <v>2</v>
       </c>
-      <c r="E2" t="n">
-        <v>7</v>
-      </c>
-      <c r="F2" t="n">
-        <v>7</v>
+      <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -504,13 +520,19 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -528,13 +550,19 @@
         </is>
       </c>
       <c r="D4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
         <v>9</v>
       </c>
-      <c r="E4" t="n">
-        <v>6</v>
-      </c>
-      <c r="F4" t="n">
-        <v>4</v>
+      <c r="G4" t="n">
+        <v>8</v>
+      </c>
+      <c r="H4" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -552,13 +580,19 @@
         </is>
       </c>
       <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
         <v>8</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>4</v>
       </c>
-      <c r="F5" t="n">
-        <v>0</v>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -576,13 +610,19 @@
         </is>
       </c>
       <c r="D6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
         <v>4</v>
       </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>8</v>
+      <c r="H6" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a Graph exersize & Made Graph 7
</commit_message>
<xml_diff>
--- a/dice_scores.xlsx
+++ b/dice_scores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,11 +474,86 @@
           <t>Round_5</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Round_6</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Round_7</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Round_8</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Round_9</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Round_10</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Round_11</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Round_12</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Round_13</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Round_14</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Round_15</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Round_16</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Round_17</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Round_18</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Round_19</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Round_20</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Altan</t>
+          <t>Yamai</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -486,29 +561,74 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Pocky Lovers</t>
+          <t>Yamai Syndicate</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2" t="n">
         <v>2</v>
-      </c>
-      <c r="G2" t="n">
-        <v>5</v>
       </c>
       <c r="H2" t="n">
         <v>4</v>
+      </c>
+      <c r="I2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J2" t="n">
+        <v>7</v>
+      </c>
+      <c r="K2" t="n">
+        <v>6</v>
+      </c>
+      <c r="L2" t="n">
+        <v>10</v>
+      </c>
+      <c r="M2" t="n">
+        <v>7</v>
+      </c>
+      <c r="N2" t="n">
+        <v>3</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>6</v>
+      </c>
+      <c r="R2" t="n">
+        <v>3</v>
+      </c>
+      <c r="S2" t="n">
+        <v>8</v>
+      </c>
+      <c r="T2" t="n">
+        <v>8</v>
+      </c>
+      <c r="U2" t="n">
+        <v>6</v>
+      </c>
+      <c r="V2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Goromi</t>
+          <t>Kalani</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -516,113 +636,68 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pocky Lovers</t>
+          <t>Yamai Syndicate</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H3" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Cyber</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+        <v>7</v>
+      </c>
+      <c r="I3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J3" t="n">
+        <v>9</v>
+      </c>
+      <c r="K3" t="n">
+        <v>4</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>6</v>
+      </c>
+      <c r="N3" t="n">
+        <v>7</v>
+      </c>
+      <c r="O3" t="n">
+        <v>10</v>
+      </c>
+      <c r="P3" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q3" t="n">
         <v>3</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Chocolate Lovers</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+      <c r="R3" t="n">
+        <v>10</v>
+      </c>
+      <c r="S3" t="n">
+        <v>3</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>6</v>
+      </c>
+      <c r="V3" t="n">
         <v>7</v>
       </c>
-      <c r="E4" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" t="n">
-        <v>9</v>
-      </c>
-      <c r="G4" t="n">
-        <v>8</v>
-      </c>
-      <c r="H4" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Nozomi</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+      <c r="W3" t="n">
         <v>4</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Chocolate Lovers</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F5" t="n">
-        <v>4</v>
-      </c>
-      <c r="G5" t="n">
-        <v>5</v>
-      </c>
-      <c r="H5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Inizio</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Pocky Lovers</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>10</v>
-      </c>
-      <c r="E6" t="n">
-        <v>10</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>4</v>
-      </c>
-      <c r="H6" t="n">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>